<commit_message>
Commit current research of memory leak into the Research Memory Management Options branch.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c51537410c5afe56/Projects/Source/Repos/SOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CA8DFEA4-113C-45AB-8D6E-41B473AE66C2}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{453C4EC4-47FF-4716-83B3-CB763E059A74}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Observations</t>
-  </si>
-  <si>
-    <t>Memory (GB)</t>
   </si>
   <si>
     <t>Question the need to store Push string in Individual object.  Why not just translate Plus program when needed.
@@ -53,6 +50,18 @@
   </si>
   <si>
     <t>Evaluated one individual on laptop with debug code single thread (break point at PushPG.compute_errors() line #38).</t>
+  </si>
+  <si>
+    <t>Heap Memory</t>
+  </si>
+  <si>
+    <t>29 GB</t>
+  </si>
+  <si>
+    <t>924.17196 GB</t>
+  </si>
+  <si>
+    <t>Evaluated one individual on desktop with debug code single thread (break point at PushPG.compute_errors() line #38).</t>
   </si>
 </sst>
 </file>
@@ -88,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -96,6 +105,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,21 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0105ADEE-4680-421E-8161-63C17F59E7EE}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="101.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -441,21 +451,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43398.458333333336</v>
       </c>
       <c r="B2" s="2">
         <v>3.2407407407407406E-2</v>
       </c>
-      <c r="C2" s="4">
-        <v>29</v>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43401.775694444441</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.3865740740740739E-2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abondoning this thread for now. Not able to get CodeBaseRegister to manage memory without memory exceptions.  Will abandon this work for now, undo the CodeBaseRegister, and continue this branch to research other options.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{453C4EC4-47FF-4716-83B3-CB763E059A74}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{F387AB10-E0D1-460B-BD8A-269F833EC03D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Evaluated one individual on desktop with debug code single thread (break point at PushPG.compute_errors() line #38).</t>
+  </si>
+  <si>
+    <t>Not able to get CodeBaseRegister to manage memory without memory exceptions.  Will abandon this work for now, undo the CodeBaseRegister, and continue this branch to research other options.</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0105ADEE-4680-421E-8161-63C17F59E7EE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,7 +434,7 @@
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="101.44140625" customWidth="1"/>
+    <col min="5" max="5" width="101.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -447,7 +450,7 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -480,6 +483,14 @@
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>43401.816666666666</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rolled-back CodeBaseRegister Removed guts of CodeBaseRegister to allow code to run without memory exceptions. Heap usage was 643,240.11 KB.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{F387AB10-E0D1-460B-BD8A-269F833EC03D}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{D48DCA4D-8225-4966-98CD-C97823E2522E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Not able to get CodeBaseRegister to manage memory without memory exceptions.  Will abandon this work for now, undo the CodeBaseRegister, and continue this branch to research other options.</t>
+  </si>
+  <si>
+    <t>643,240.11 KB</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0105ADEE-4680-421E-8161-63C17F59E7EE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +496,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>43401.843055555553</v>
+      </c>
+      <c r="B5" s="5">
+        <v>9.8379629629629633E-3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Memory Benchmark = 255,320,430 bytes
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{D48DCA4D-8225-4966-98CD-C97823E2522E}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{6737050E-805C-484B-ACB9-A62706374D2B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VS Heap Tool" sheetId="1" r:id="rId1"/>
+    <sheet name="Heap Report from Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +69,33 @@
   </si>
   <si>
     <t>643,240.11 KB</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 1</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 2</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 3</t>
+  </si>
+  <si>
+    <t>Research_Memory_Management_Options</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Release</t>
   </si>
 </sst>
 </file>
@@ -428,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0105ADEE-4680-421E-8161-63C17F59E7EE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,4 +542,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="50.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43409.84375</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>255320430</v>
+      </c>
+      <c r="G2" s="4">
+        <v>255320430</v>
+      </c>
+      <c r="H2" s="4">
+        <v>255320430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Memory Benchmark Sometimes better, sometimes worse.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{D48DCA4D-8225-4966-98CD-C97823E2522E}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{2E92929C-EAF5-4797-A215-059192303CE9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VS Heap Tool" sheetId="1" r:id="rId1"/>
+    <sheet name="Heap Report from Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +69,36 @@
   </si>
   <si>
     <t>643,240.11 KB</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 1</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 2</t>
+  </si>
+  <si>
+    <t>Heap Memory Test 3</t>
+  </si>
+  <si>
+    <t>Research_Memory_Management_Options</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Factory_Class</t>
   </si>
 </sst>
 </file>
@@ -428,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0105ADEE-4680-421E-8161-63C17F59E7EE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,4 +545,104 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="50.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>43409.84375</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>255320430</v>
+      </c>
+      <c r="G2" s="4">
+        <v>255320430</v>
+      </c>
+      <c r="H2" s="4">
+        <v>255320430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>43409.854166666664</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4">
+        <v>83737598</v>
+      </c>
+      <c r="G3" s="4">
+        <v>190402070</v>
+      </c>
+      <c r="H3" s="4">
+        <v>403696526</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[WIP] PushP Memory Usage = 130,095
Limited test to PushP.  Also, updated pack() in Literal.h to use factory.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{2E92929C-EAF5-4797-A215-059192303CE9}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{93548474-4F70-4B03-9F70-681175152695}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
   <sheets>
     <sheet name="VS Heap Tool" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>Factory_Class</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Memory usage seems random between 83M and 403M</t>
+  </si>
+  <si>
+    <t>Full test of PushP and PushGP.</t>
+  </si>
+  <si>
+    <t>Limited test to PushP.  Also, updated pack() in Literal.h to use factory.</t>
+  </si>
+  <si>
+    <t>Memory usage consistant</t>
   </si>
 </sst>
 </file>
@@ -463,15 +478,15 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="101.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43398.458333333336</v>
       </c>
@@ -505,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43401.775694444441</v>
       </c>
@@ -519,7 +534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43401.816666666666</v>
       </c>
@@ -527,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43401.843055555553</v>
       </c>
@@ -549,21 +564,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="50.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43409.84375</v>
       </c>
@@ -618,7 +633,7 @@
         <v>255320430</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43409.854166666664</v>
       </c>
@@ -639,6 +654,41 @@
       </c>
       <c r="H3" s="4">
         <v>403696526</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43411.40625</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="4">
+        <v>130095</v>
+      </c>
+      <c r="G4" s="4">
+        <v>130095</v>
+      </c>
+      <c r="H4" s="4">
+        <v>130095</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] PushP Memory Usage = 130,007
Replaced adopt() in Code.h with call to CodeList() constructor.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{93548474-4F70-4B03-9F70-681175152695}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{16D8AC63-D989-4336-9E37-78599DD3025C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Memory usage consistant</t>
+  </si>
+  <si>
+    <t>Replaced adopt() in Code.h with call to CodeList() constructor</t>
   </si>
 </sst>
 </file>
@@ -564,11 +567,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -691,6 +692,32 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43411.458333333336</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4">
+        <v>130007</v>
+      </c>
+      <c r="G5" s="4">
+        <v>130007</v>
+      </c>
+      <c r="H5" s="4">
+        <v>130007</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
[WIP] PushP Memory Usage = 116,791
Implemented CodeList Heap Manager.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{16D8AC63-D989-4336-9E37-78599DD3025C}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{AD31A966-F7D6-4DCA-AB36-532D14E658FE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Replaced adopt() in Code.h with call to CodeList() constructor</t>
+  </si>
+  <si>
+    <t>Implemented CodeList Heap Manager</t>
   </si>
 </sst>
 </file>
@@ -567,9 +570,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -718,6 +723,32 @@
         <v>27</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43411.020833333336</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4">
+        <v>116791</v>
+      </c>
+      <c r="G6" s="4">
+        <v>116791</v>
+      </c>
+      <c r="H6" s="4">
+        <v>116791</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
[WIP] PushP Memory Usage = 16
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarrity\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{AD31A966-F7D6-4DCA-AB36-532D14E658FE}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="8_{63BF45B0-FA21-4463-8234-338C77BF610A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{06F2E473-0FF6-4A0E-AD16-2EA1A08A6352}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Implemented CodeList Heap Manager</t>
+  </si>
+  <si>
+    <t>Consolidated creation of static Push code snippets</t>
   </si>
 </sst>
 </file>
@@ -570,11 +573,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -749,6 +750,32 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43412.73333333333</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4">
+        <v>16</v>
+      </c>
+      <c r="H7" s="4">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Reserved max_point_evaluations on the stacks.  Did not seem to make a difference in the memory usage.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="102_{9866D328-2DCF-483C-B536-09158372D0B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="102_{9866D328-2DCF-483C-B536-09158372D0B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{454EDCEC-195C-4ACD-B791-232AD167801B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,19 @@
   <si>
     <t>382,852
 385,492</t>
+  </si>
+  <si>
+    <t>Reserve_Stack_Space</t>
+  </si>
+  <si>
+    <t>7,916
+7,916
+7,916</t>
+  </si>
+  <si>
+    <t>42,292
+42,132
+42,372</t>
   </si>
 </sst>
 </file>
@@ -252,8 +265,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3BBB98D-4CE1-4005-A70E-9981EE0DA113}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:J10" xr:uid="{FC87183D-D316-48E5-9B11-07D68CBF7FC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3BBB98D-4CE1-4005-A70E-9981EE0DA113}" name="Table1" displayName="Table1" ref="A1:J11" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:J11" xr:uid="{FC87183D-D316-48E5-9B11-07D68CBF7FC6}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3CC0C68B-B0DE-46DB-9383-B12F059046F8}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{12D948F6-6D3F-4408-AF4B-8CD963811641}" name="Platform"/>
@@ -659,11 +672,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -944,6 +955,28 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>43426.651388888888</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Average memory usage for 1000 iterations is 384,105 bytes.
</commit_message>
<xml_diff>
--- a/Analysis.xlsx
+++ b/Analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\OneDrive\Projects\Source\Repos\EdGarrity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="102_{9866D328-2DCF-483C-B536-09158372D0B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="102_{DAFD78B7-958E-41FD-9EC5-EE13054F3160}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{125419F0-DA63-4FF7-989D-088428572D7A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{A1EEA105-3448-413D-A0DE-C59B297D242E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,38 @@
   <si>
     <t>382,852
 385,492</t>
+  </si>
+  <si>
+    <t>Reserve_Stack_Space</t>
+  </si>
+  <si>
+    <t>7,916
+7,916
+7,916</t>
+  </si>
+  <si>
+    <t>42,292
+42,132
+42,372</t>
+  </si>
+  <si>
+    <t>42,612
+42,852
+42,692</t>
+  </si>
+  <si>
+    <t>382,452
+385,252
+384,612</t>
+  </si>
+  <si>
+    <t>Average memory usage for 1000 iterations is 384,105 bytes.</t>
+  </si>
+  <si>
+    <t>Merged updates from the Factory_Class branch.</t>
+  </si>
+  <si>
+    <t>No difference</t>
   </si>
 </sst>
 </file>
@@ -252,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3BBB98D-4CE1-4005-A70E-9981EE0DA113}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:J10" xr:uid="{FC87183D-D316-48E5-9B11-07D68CBF7FC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3BBB98D-4CE1-4005-A70E-9981EE0DA113}" name="Table1" displayName="Table1" ref="A1:J12" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:J12" xr:uid="{FC87183D-D316-48E5-9B11-07D68CBF7FC6}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3CC0C68B-B0DE-46DB-9383-B12F059046F8}" name="Date" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{12D948F6-6D3F-4408-AF4B-8CD963811641}" name="Platform"/>
@@ -659,10 +691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8A60E5-87A9-419C-8F76-5A9AAC406F60}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,6 +976,60 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>43426.651388888888</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>43427.679861111108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>